<commit_message>
Moved sqlite table creation from signup to signup confirm
</commit_message>
<xml_diff>
--- a/FYP documentation/FYP_Project_Plan.xlsx
+++ b/FYP documentation/FYP_Project_Plan.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18431"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18528"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -614,17 +614,89 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="1" xfId="7" applyFont="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="15" fillId="6" borderId="1" xfId="13" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="4" xfId="14" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="3" xfId="15" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="3" xfId="16" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="3" xfId="17" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="3" xfId="18" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="11" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="17" fillId="0" borderId="2" xfId="3" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="20" fillId="0" borderId="0" xfId="6" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="2" applyFont="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="2" applyFont="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="22" fillId="0" borderId="0" xfId="6" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="12" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="1" xfId="7" applyFont="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="15" fillId="6" borderId="1" xfId="13" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="4" xfId="14" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="9" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="9" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="10" applyFont="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="10" applyFont="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="10" applyFont="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="10" applyFont="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
@@ -635,27 +707,12 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="3" xfId="15" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="3" xfId="16" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="3" xfId="17" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -664,63 +721,6 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="3" xfId="18" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="9" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="10" applyFont="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="10" applyFont="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="11" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="9" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="10" applyFont="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="10" applyFont="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="17" fillId="0" borderId="2" xfId="3" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="20" fillId="0" borderId="0" xfId="6" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="2" applyFont="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="2" applyFont="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="22" fillId="0" borderId="0" xfId="6" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -1133,16 +1133,16 @@
   </sheetPr>
   <dimension ref="B1:GD38"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="59" zoomScaleNormal="59" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" zoomScale="59" zoomScaleNormal="59" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="2.6640625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="36.6640625" style="39" customWidth="1"/>
+    <col min="2" max="2" width="36.6640625" style="22" customWidth="1"/>
     <col min="3" max="6" width="11.6640625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="15.6640625" style="40" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" style="23" customWidth="1"/>
     <col min="8" max="8" width="3.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="9" max="23" width="2.77734375" style="3"/>
     <col min="24" max="24" width="12" style="3" customWidth="1"/>
@@ -1163,1179 +1163,1193 @@
       <c r="G1" s="2"/>
     </row>
     <row r="2" spans="2:186" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="6" t="s">
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="7">
+      <c r="H2" s="6">
         <v>85</v>
       </c>
-      <c r="J2" s="8"/>
-      <c r="K2" s="9" t="s">
+      <c r="J2" s="7"/>
+      <c r="K2" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10"/>
-      <c r="N2" s="10"/>
-      <c r="O2" s="11"/>
-      <c r="P2" s="12"/>
-      <c r="Q2" s="9" t="s">
+      <c r="L2" s="34"/>
+      <c r="M2" s="34"/>
+      <c r="N2" s="34"/>
+      <c r="O2" s="35"/>
+      <c r="P2" s="8"/>
+      <c r="Q2" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="R2" s="13"/>
-      <c r="S2" s="13"/>
-      <c r="T2" s="11"/>
-      <c r="U2" s="14"/>
-      <c r="V2" s="15" t="s">
+      <c r="R2" s="36"/>
+      <c r="S2" s="36"/>
+      <c r="T2" s="35"/>
+      <c r="U2" s="9"/>
+      <c r="V2" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="W2" s="16"/>
-      <c r="X2" s="16"/>
-      <c r="Y2" s="17"/>
-      <c r="Z2" s="18"/>
-      <c r="AA2" s="19" t="s">
+      <c r="W2" s="25"/>
+      <c r="X2" s="25"/>
+      <c r="Y2" s="37"/>
+      <c r="Z2" s="10"/>
+      <c r="AA2" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="AB2" s="20"/>
-      <c r="AC2" s="20"/>
-      <c r="AD2" s="20"/>
-      <c r="AE2" s="20"/>
-      <c r="AF2" s="20"/>
-      <c r="AG2" s="21"/>
-      <c r="AH2" s="22"/>
-      <c r="AI2" s="15" t="s">
+      <c r="AB2" s="39"/>
+      <c r="AC2" s="39"/>
+      <c r="AD2" s="39"/>
+      <c r="AE2" s="39"/>
+      <c r="AF2" s="39"/>
+      <c r="AG2" s="40"/>
+      <c r="AH2" s="11"/>
+      <c r="AI2" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="AJ2" s="16"/>
-      <c r="AK2" s="16"/>
-      <c r="AL2" s="16"/>
-      <c r="AM2" s="16"/>
-      <c r="AN2" s="16"/>
-      <c r="AO2" s="16"/>
-      <c r="AP2" s="16"/>
-    </row>
-    <row r="3" spans="2:186" s="29" customFormat="1" ht="39.9" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="24" t="s">
+      <c r="AJ2" s="25"/>
+      <c r="AK2" s="25"/>
+      <c r="AL2" s="25"/>
+      <c r="AM2" s="25"/>
+      <c r="AN2" s="25"/>
+      <c r="AO2" s="25"/>
+      <c r="AP2" s="25"/>
+    </row>
+    <row r="3" spans="2:186" s="15" customFormat="1" ht="39.9" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="24" t="s">
+      <c r="D3" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="24" t="s">
+      <c r="E3" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="24" t="s">
+      <c r="F3" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="25" t="s">
+      <c r="G3" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="26" t="s">
+      <c r="H3" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="I3" s="27"/>
-      <c r="J3" s="28"/>
-      <c r="K3" s="28"/>
-      <c r="L3" s="28"/>
-      <c r="M3" s="28"/>
-      <c r="N3" s="28"/>
-      <c r="O3" s="28"/>
-      <c r="P3" s="28"/>
-      <c r="Q3" s="28"/>
-      <c r="R3" s="28"/>
-      <c r="S3" s="28"/>
-      <c r="T3" s="28"/>
-      <c r="U3" s="28"/>
-      <c r="V3" s="28"/>
-      <c r="W3" s="28"/>
-      <c r="X3" s="28"/>
-      <c r="Y3" s="28"/>
-      <c r="Z3" s="28"/>
-      <c r="AA3" s="28"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="14"/>
+      <c r="O3" s="14"/>
+      <c r="P3" s="14"/>
+      <c r="Q3" s="14"/>
+      <c r="R3" s="14"/>
+      <c r="S3" s="14"/>
+      <c r="T3" s="14"/>
+      <c r="U3" s="14"/>
+      <c r="V3" s="14"/>
+      <c r="W3" s="14"/>
+      <c r="X3" s="14"/>
+      <c r="Y3" s="14"/>
+      <c r="Z3" s="14"/>
+      <c r="AA3" s="14"/>
     </row>
     <row r="4" spans="2:186" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="30"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
+      <c r="B4" s="28"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
       <c r="G4" s="32"/>
-      <c r="H4" s="33">
-        <v>1</v>
-      </c>
-      <c r="I4" s="33">
+      <c r="H4" s="16">
+        <v>1</v>
+      </c>
+      <c r="I4" s="16">
         <v>2</v>
       </c>
-      <c r="J4" s="33">
+      <c r="J4" s="16">
         <v>3</v>
       </c>
-      <c r="K4" s="33">
+      <c r="K4" s="16">
         <v>4</v>
       </c>
-      <c r="L4" s="33">
+      <c r="L4" s="16">
         <v>5</v>
       </c>
-      <c r="M4" s="33">
+      <c r="M4" s="16">
         <v>6</v>
       </c>
-      <c r="N4" s="33">
+      <c r="N4" s="16">
         <v>7</v>
       </c>
-      <c r="O4" s="33">
+      <c r="O4" s="16">
         <v>8</v>
       </c>
-      <c r="P4" s="33">
+      <c r="P4" s="16">
         <v>9</v>
       </c>
-      <c r="Q4" s="33">
+      <c r="Q4" s="16">
         <v>10</v>
       </c>
-      <c r="R4" s="33">
+      <c r="R4" s="16">
         <v>11</v>
       </c>
-      <c r="S4" s="33">
+      <c r="S4" s="16">
         <v>12</v>
       </c>
-      <c r="T4" s="33">
+      <c r="T4" s="16">
         <v>13</v>
       </c>
-      <c r="U4" s="33">
+      <c r="U4" s="16">
         <v>14</v>
       </c>
-      <c r="V4" s="33">
+      <c r="V4" s="16">
         <v>15</v>
       </c>
-      <c r="W4" s="33">
+      <c r="W4" s="16">
         <v>16</v>
       </c>
-      <c r="X4" s="33">
+      <c r="X4" s="16">
         <v>17</v>
       </c>
-      <c r="Y4" s="33">
+      <c r="Y4" s="16">
         <v>18</v>
       </c>
-      <c r="Z4" s="33">
+      <c r="Z4" s="16">
         <v>19</v>
       </c>
-      <c r="AA4" s="33">
+      <c r="AA4" s="16">
         <v>20</v>
       </c>
-      <c r="AB4" s="33">
+      <c r="AB4" s="16">
         <v>21</v>
       </c>
-      <c r="AC4" s="33">
+      <c r="AC4" s="16">
         <v>22</v>
       </c>
-      <c r="AD4" s="33">
+      <c r="AD4" s="16">
         <v>23</v>
       </c>
-      <c r="AE4" s="33">
+      <c r="AE4" s="16">
         <v>24</v>
       </c>
-      <c r="AF4" s="33">
+      <c r="AF4" s="16">
         <v>25</v>
       </c>
-      <c r="AG4" s="33">
+      <c r="AG4" s="16">
         <v>26</v>
       </c>
-      <c r="AH4" s="33">
+      <c r="AH4" s="16">
         <v>27</v>
       </c>
-      <c r="AI4" s="33">
+      <c r="AI4" s="16">
         <v>28</v>
       </c>
-      <c r="AJ4" s="33">
+      <c r="AJ4" s="16">
         <v>29</v>
       </c>
-      <c r="AK4" s="33">
+      <c r="AK4" s="16">
         <v>30</v>
       </c>
-      <c r="AL4" s="33">
+      <c r="AL4" s="16">
         <v>31</v>
       </c>
-      <c r="AM4" s="33">
+      <c r="AM4" s="16">
         <v>32</v>
       </c>
-      <c r="AN4" s="33">
+      <c r="AN4" s="16">
         <v>33</v>
       </c>
-      <c r="AO4" s="33">
+      <c r="AO4" s="16">
         <v>34</v>
       </c>
-      <c r="AP4" s="33">
+      <c r="AP4" s="16">
         <v>35</v>
       </c>
-      <c r="AQ4" s="33">
+      <c r="AQ4" s="16">
         <v>36</v>
       </c>
-      <c r="AR4" s="33">
+      <c r="AR4" s="16">
         <v>37</v>
       </c>
-      <c r="AS4" s="33">
+      <c r="AS4" s="16">
         <v>38</v>
       </c>
-      <c r="AT4" s="33">
+      <c r="AT4" s="16">
         <v>39</v>
       </c>
-      <c r="AU4" s="33">
+      <c r="AU4" s="16">
         <v>40</v>
       </c>
-      <c r="AV4" s="33">
+      <c r="AV4" s="16">
         <v>41</v>
       </c>
-      <c r="AW4" s="33">
+      <c r="AW4" s="16">
         <v>42</v>
       </c>
-      <c r="AX4" s="33">
+      <c r="AX4" s="16">
         <v>43</v>
       </c>
-      <c r="AY4" s="33">
+      <c r="AY4" s="16">
         <v>44</v>
       </c>
-      <c r="AZ4" s="33">
+      <c r="AZ4" s="16">
         <v>45</v>
       </c>
-      <c r="BA4" s="33">
+      <c r="BA4" s="16">
         <v>46</v>
       </c>
-      <c r="BB4" s="33">
+      <c r="BB4" s="16">
         <v>47</v>
       </c>
-      <c r="BC4" s="33">
+      <c r="BC4" s="16">
         <v>48</v>
       </c>
-      <c r="BD4" s="33">
+      <c r="BD4" s="16">
         <v>49</v>
       </c>
-      <c r="BE4" s="33">
+      <c r="BE4" s="16">
         <v>50</v>
       </c>
-      <c r="BF4" s="33">
+      <c r="BF4" s="16">
         <v>51</v>
       </c>
-      <c r="BG4" s="33">
+      <c r="BG4" s="16">
         <v>52</v>
       </c>
-      <c r="BH4" s="33">
+      <c r="BH4" s="16">
         <v>53</v>
       </c>
-      <c r="BI4" s="33">
+      <c r="BI4" s="16">
         <v>54</v>
       </c>
-      <c r="BJ4" s="33">
+      <c r="BJ4" s="16">
         <v>55</v>
       </c>
-      <c r="BK4" s="33">
+      <c r="BK4" s="16">
         <v>56</v>
       </c>
-      <c r="BL4" s="33">
+      <c r="BL4" s="16">
         <v>57</v>
       </c>
-      <c r="BM4" s="33">
+      <c r="BM4" s="16">
         <v>58</v>
       </c>
-      <c r="BN4" s="33">
+      <c r="BN4" s="16">
         <v>59</v>
       </c>
-      <c r="BO4" s="33">
+      <c r="BO4" s="16">
         <v>60</v>
       </c>
-      <c r="BP4" s="33">
+      <c r="BP4" s="16">
         <v>61</v>
       </c>
-      <c r="BQ4" s="33">
+      <c r="BQ4" s="16">
         <v>62</v>
       </c>
-      <c r="BR4" s="33">
+      <c r="BR4" s="16">
         <v>63</v>
       </c>
-      <c r="BS4" s="33">
+      <c r="BS4" s="16">
         <v>64</v>
       </c>
-      <c r="BT4" s="33">
+      <c r="BT4" s="16">
         <v>65</v>
       </c>
-      <c r="BU4" s="33">
+      <c r="BU4" s="16">
         <v>66</v>
       </c>
-      <c r="BV4" s="33">
+      <c r="BV4" s="16">
         <v>67</v>
       </c>
-      <c r="BW4" s="33">
+      <c r="BW4" s="16">
         <v>68</v>
       </c>
-      <c r="BX4" s="33">
+      <c r="BX4" s="16">
         <v>69</v>
       </c>
-      <c r="BY4" s="33">
+      <c r="BY4" s="16">
         <v>70</v>
       </c>
-      <c r="BZ4" s="33">
+      <c r="BZ4" s="16">
         <v>71</v>
       </c>
-      <c r="CA4" s="33">
+      <c r="CA4" s="16">
         <v>72</v>
       </c>
-      <c r="CB4" s="33">
+      <c r="CB4" s="16">
         <v>73</v>
       </c>
-      <c r="CC4" s="33">
+      <c r="CC4" s="16">
         <v>74</v>
       </c>
-      <c r="CD4" s="33">
+      <c r="CD4" s="16">
         <v>75</v>
       </c>
-      <c r="CE4" s="33">
+      <c r="CE4" s="16">
         <v>76</v>
       </c>
-      <c r="CF4" s="33">
+      <c r="CF4" s="16">
         <v>77</v>
       </c>
-      <c r="CG4" s="33">
+      <c r="CG4" s="16">
         <v>78</v>
       </c>
-      <c r="CH4" s="33">
+      <c r="CH4" s="16">
         <v>79</v>
       </c>
-      <c r="CI4" s="33">
+      <c r="CI4" s="16">
         <v>80</v>
       </c>
-      <c r="CJ4" s="33">
+      <c r="CJ4" s="16">
         <v>81</v>
       </c>
-      <c r="CK4" s="33">
+      <c r="CK4" s="16">
         <v>82</v>
       </c>
-      <c r="CL4" s="33">
+      <c r="CL4" s="16">
         <v>83</v>
       </c>
-      <c r="CM4" s="33">
+      <c r="CM4" s="16">
         <v>84</v>
       </c>
-      <c r="CN4" s="33">
+      <c r="CN4" s="16">
         <v>85</v>
       </c>
-      <c r="CO4" s="33">
+      <c r="CO4" s="16">
         <v>86</v>
       </c>
-      <c r="CP4" s="33">
+      <c r="CP4" s="16">
         <v>87</v>
       </c>
-      <c r="CQ4" s="33">
+      <c r="CQ4" s="16">
         <v>88</v>
       </c>
-      <c r="CR4" s="33">
+      <c r="CR4" s="16">
         <v>89</v>
       </c>
-      <c r="CS4" s="33">
+      <c r="CS4" s="16">
         <v>90</v>
       </c>
-      <c r="CT4" s="33">
+      <c r="CT4" s="16">
         <v>91</v>
       </c>
-      <c r="CU4" s="33">
+      <c r="CU4" s="16">
         <v>92</v>
       </c>
-      <c r="CV4" s="33">
+      <c r="CV4" s="16">
         <v>93</v>
       </c>
-      <c r="CW4" s="33">
+      <c r="CW4" s="16">
         <v>94</v>
       </c>
-      <c r="CX4" s="33">
+      <c r="CX4" s="16">
         <v>95</v>
       </c>
-      <c r="CY4" s="33">
+      <c r="CY4" s="16">
         <v>96</v>
       </c>
-      <c r="CZ4" s="33">
+      <c r="CZ4" s="16">
         <v>97</v>
       </c>
-      <c r="DA4" s="33">
+      <c r="DA4" s="16">
         <v>98</v>
       </c>
-      <c r="DB4" s="33">
+      <c r="DB4" s="16">
         <v>99</v>
       </c>
-      <c r="DC4" s="33">
+      <c r="DC4" s="16">
         <v>100</v>
       </c>
-      <c r="DD4" s="33">
+      <c r="DD4" s="16">
         <v>101</v>
       </c>
-      <c r="DE4" s="33">
+      <c r="DE4" s="16">
         <v>102</v>
       </c>
-      <c r="DF4" s="33">
+      <c r="DF4" s="16">
         <v>103</v>
       </c>
-      <c r="DG4" s="33">
+      <c r="DG4" s="16">
         <v>104</v>
       </c>
-      <c r="DH4" s="33">
+      <c r="DH4" s="16">
         <v>105</v>
       </c>
-      <c r="DI4" s="33">
+      <c r="DI4" s="16">
         <v>106</v>
       </c>
-      <c r="DJ4" s="33">
+      <c r="DJ4" s="16">
         <v>107</v>
       </c>
-      <c r="DK4" s="33">
+      <c r="DK4" s="16">
         <v>108</v>
       </c>
-      <c r="DL4" s="33">
+      <c r="DL4" s="16">
         <v>109</v>
       </c>
-      <c r="DM4" s="33">
+      <c r="DM4" s="16">
         <v>110</v>
       </c>
-      <c r="DN4" s="33">
+      <c r="DN4" s="16">
         <v>111</v>
       </c>
-      <c r="DO4" s="33">
+      <c r="DO4" s="16">
         <v>112</v>
       </c>
-      <c r="DP4" s="33">
+      <c r="DP4" s="16">
         <v>113</v>
       </c>
-      <c r="DQ4" s="33">
+      <c r="DQ4" s="16">
         <v>114</v>
       </c>
-      <c r="DR4" s="33">
+      <c r="DR4" s="16">
         <v>115</v>
       </c>
-      <c r="DS4" s="33">
+      <c r="DS4" s="16">
         <v>116</v>
       </c>
-      <c r="DT4" s="33">
+      <c r="DT4" s="16">
         <v>117</v>
       </c>
-      <c r="DU4" s="33">
+      <c r="DU4" s="16">
         <v>118</v>
       </c>
-      <c r="DV4" s="33">
+      <c r="DV4" s="16">
         <v>119</v>
       </c>
-      <c r="DW4" s="33">
+      <c r="DW4" s="16">
         <v>120</v>
       </c>
-      <c r="DX4" s="33">
+      <c r="DX4" s="16">
         <v>121</v>
       </c>
-      <c r="DY4" s="33">
+      <c r="DY4" s="16">
         <v>122</v>
       </c>
-      <c r="DZ4" s="33">
+      <c r="DZ4" s="16">
         <v>123</v>
       </c>
-      <c r="EA4" s="33">
+      <c r="EA4" s="16">
         <v>124</v>
       </c>
-      <c r="EB4" s="33">
+      <c r="EB4" s="16">
         <v>125</v>
       </c>
-      <c r="EC4" s="33">
+      <c r="EC4" s="16">
         <v>126</v>
       </c>
-      <c r="ED4" s="33">
+      <c r="ED4" s="16">
         <v>127</v>
       </c>
-      <c r="EE4" s="33">
+      <c r="EE4" s="16">
         <v>128</v>
       </c>
-      <c r="EF4" s="33">
+      <c r="EF4" s="16">
         <v>129</v>
       </c>
-      <c r="EG4" s="33">
+      <c r="EG4" s="16">
         <v>130</v>
       </c>
-      <c r="EH4" s="33">
+      <c r="EH4" s="16">
         <v>131</v>
       </c>
-      <c r="EI4" s="33">
+      <c r="EI4" s="16">
         <v>132</v>
       </c>
-      <c r="EJ4" s="33">
+      <c r="EJ4" s="16">
         <v>133</v>
       </c>
-      <c r="EK4" s="33">
+      <c r="EK4" s="16">
         <v>134</v>
       </c>
-      <c r="EL4" s="33">
+      <c r="EL4" s="16">
         <v>135</v>
       </c>
-      <c r="EM4" s="33">
+      <c r="EM4" s="16">
         <v>136</v>
       </c>
-      <c r="EN4" s="33">
+      <c r="EN4" s="16">
         <v>137</v>
       </c>
-      <c r="EO4" s="33">
+      <c r="EO4" s="16">
         <v>138</v>
       </c>
-      <c r="EP4" s="33">
+      <c r="EP4" s="16">
         <v>139</v>
       </c>
-      <c r="EQ4" s="33">
+      <c r="EQ4" s="16">
         <v>140</v>
       </c>
-      <c r="ER4" s="33">
+      <c r="ER4" s="16">
         <v>141</v>
       </c>
-      <c r="ES4" s="33">
+      <c r="ES4" s="16">
         <v>142</v>
       </c>
-      <c r="ET4" s="33">
+      <c r="ET4" s="16">
         <v>143</v>
       </c>
-      <c r="EU4" s="33">
+      <c r="EU4" s="16">
         <v>144</v>
       </c>
-      <c r="EV4" s="33">
+      <c r="EV4" s="16">
         <v>145</v>
       </c>
-      <c r="EW4" s="33">
+      <c r="EW4" s="16">
         <v>146</v>
       </c>
-      <c r="EX4" s="33">
+      <c r="EX4" s="16">
         <v>147</v>
       </c>
-      <c r="EY4" s="33">
+      <c r="EY4" s="16">
         <v>148</v>
       </c>
-      <c r="EZ4" s="33">
+      <c r="EZ4" s="16">
         <v>149</v>
       </c>
-      <c r="FA4" s="33">
+      <c r="FA4" s="16">
         <v>150</v>
       </c>
-      <c r="FB4" s="33">
+      <c r="FB4" s="16">
         <v>151</v>
       </c>
-      <c r="FC4" s="33">
+      <c r="FC4" s="16">
         <v>152</v>
       </c>
-      <c r="FD4" s="33">
+      <c r="FD4" s="16">
         <v>153</v>
       </c>
-      <c r="FE4" s="33">
+      <c r="FE4" s="16">
         <v>154</v>
       </c>
-      <c r="FF4" s="33">
+      <c r="FF4" s="16">
         <v>155</v>
       </c>
-      <c r="FG4" s="33">
+      <c r="FG4" s="16">
         <v>156</v>
       </c>
-      <c r="FH4" s="33">
+      <c r="FH4" s="16">
         <v>157</v>
       </c>
-      <c r="FI4" s="33">
+      <c r="FI4" s="16">
         <v>158</v>
       </c>
-      <c r="FJ4" s="33">
+      <c r="FJ4" s="16">
         <v>159</v>
       </c>
-      <c r="FK4" s="33">
+      <c r="FK4" s="16">
         <v>160</v>
       </c>
-      <c r="FL4" s="33">
+      <c r="FL4" s="16">
         <v>161</v>
       </c>
-      <c r="FM4" s="33">
+      <c r="FM4" s="16">
         <v>162</v>
       </c>
-      <c r="FN4" s="33">
+      <c r="FN4" s="16">
         <v>163</v>
       </c>
-      <c r="FO4" s="33">
+      <c r="FO4" s="16">
         <v>164</v>
       </c>
-      <c r="FP4" s="33">
+      <c r="FP4" s="16">
         <v>165</v>
       </c>
-      <c r="FQ4" s="33">
+      <c r="FQ4" s="16">
         <v>166</v>
       </c>
-      <c r="FR4" s="33">
+      <c r="FR4" s="16">
         <v>167</v>
       </c>
-      <c r="FS4" s="33">
+      <c r="FS4" s="16">
         <v>168</v>
       </c>
-      <c r="FT4" s="33">
+      <c r="FT4" s="16">
         <v>169</v>
       </c>
-      <c r="FU4" s="33">
+      <c r="FU4" s="16">
         <v>170</v>
       </c>
-      <c r="FV4" s="33">
+      <c r="FV4" s="16">
         <v>171</v>
       </c>
-      <c r="FW4" s="33">
+      <c r="FW4" s="16">
         <v>172</v>
       </c>
-      <c r="FX4" s="33">
+      <c r="FX4" s="16">
         <v>173</v>
       </c>
-      <c r="FY4" s="33">
+      <c r="FY4" s="16">
         <v>174</v>
       </c>
-      <c r="FZ4" s="33">
+      <c r="FZ4" s="16">
         <v>175</v>
       </c>
-      <c r="GA4" s="33">
+      <c r="GA4" s="16">
         <v>176</v>
       </c>
-      <c r="GB4" s="33">
+      <c r="GB4" s="16">
         <v>177</v>
       </c>
-      <c r="GC4" s="33">
+      <c r="GC4" s="16">
         <v>178</v>
       </c>
-      <c r="GD4" s="33">
+      <c r="GD4" s="16">
         <v>179</v>
       </c>
     </row>
     <row r="5" spans="2:186" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="35">
-        <v>1</v>
-      </c>
-      <c r="D5" s="35">
+      <c r="C5" s="18">
+        <v>1</v>
+      </c>
+      <c r="D5" s="18">
         <v>15</v>
       </c>
-      <c r="E5" s="35">
-        <v>1</v>
-      </c>
-      <c r="F5" s="35">
+      <c r="E5" s="18">
+        <v>1</v>
+      </c>
+      <c r="F5" s="18">
         <v>16</v>
       </c>
-      <c r="G5" s="36">
+      <c r="G5" s="19">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="2:186" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="34" t="s">
+      <c r="B6" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="35">
-        <v>1</v>
-      </c>
-      <c r="D6" s="35">
+      <c r="C6" s="18">
+        <v>1</v>
+      </c>
+      <c r="D6" s="18">
         <v>2</v>
       </c>
-      <c r="E6" s="35">
-        <v>1</v>
-      </c>
-      <c r="F6" s="35">
+      <c r="E6" s="18">
+        <v>1</v>
+      </c>
+      <c r="F6" s="18">
         <v>2</v>
       </c>
-      <c r="G6" s="36">
+      <c r="G6" s="19">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="2:186" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="35">
+      <c r="C7" s="18">
         <v>4</v>
       </c>
-      <c r="D7" s="35">
+      <c r="D7" s="18">
         <v>2</v>
       </c>
-      <c r="E7" s="35">
+      <c r="E7" s="18">
         <v>4</v>
       </c>
-      <c r="F7" s="35">
+      <c r="F7" s="18">
         <v>2</v>
       </c>
-      <c r="G7" s="36">
+      <c r="G7" s="19">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="2:186" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="35">
+      <c r="C8" s="18">
         <v>6</v>
       </c>
-      <c r="D8" s="35">
+      <c r="D8" s="18">
         <v>2</v>
       </c>
-      <c r="E8" s="35">
+      <c r="E8" s="18">
         <v>6</v>
       </c>
-      <c r="F8" s="35">
+      <c r="F8" s="18">
         <v>2</v>
       </c>
-      <c r="G8" s="36">
+      <c r="G8" s="19">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="2:186" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="34" t="s">
+      <c r="B9" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="35">
+      <c r="C9" s="18">
         <v>8</v>
       </c>
-      <c r="D9" s="35">
+      <c r="D9" s="18">
         <v>2</v>
       </c>
-      <c r="E9" s="35">
+      <c r="E9" s="18">
         <v>8</v>
       </c>
-      <c r="F9" s="35">
+      <c r="F9" s="18">
         <v>2</v>
       </c>
-      <c r="G9" s="36">
+      <c r="G9" s="19">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="2:186" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="34" t="s">
+      <c r="B10" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="35">
+      <c r="C10" s="18">
         <v>10</v>
       </c>
-      <c r="D10" s="35">
+      <c r="D10" s="18">
         <v>2</v>
       </c>
-      <c r="E10" s="35">
+      <c r="E10" s="18">
         <v>10</v>
       </c>
-      <c r="F10" s="35">
+      <c r="F10" s="18">
         <v>3</v>
       </c>
-      <c r="G10" s="36">
+      <c r="G10" s="19">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="2:186" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="34" t="s">
+      <c r="B11" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="35">
+      <c r="C11" s="18">
         <v>12</v>
       </c>
-      <c r="D11" s="35">
+      <c r="D11" s="18">
         <v>3</v>
       </c>
-      <c r="E11" s="35">
+      <c r="E11" s="18">
         <v>13</v>
       </c>
-      <c r="F11" s="35">
+      <c r="F11" s="18">
         <v>3</v>
       </c>
-      <c r="G11" s="36">
+      <c r="G11" s="19">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="2:186" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="34" t="s">
+      <c r="B12" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="35">
+      <c r="C12" s="18">
         <v>16</v>
       </c>
-      <c r="D12" s="35">
+      <c r="D12" s="18">
         <v>13</v>
       </c>
-      <c r="E12" s="35">
+      <c r="E12" s="18">
         <v>17</v>
       </c>
-      <c r="F12" s="35">
+      <c r="F12" s="18">
         <v>13</v>
       </c>
-      <c r="G12" s="36">
+      <c r="G12" s="19">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="2:186" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="34" t="s">
+      <c r="B13" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="35">
+      <c r="C13" s="18">
         <v>16</v>
       </c>
-      <c r="D13" s="35">
+      <c r="D13" s="18">
         <v>3</v>
       </c>
-      <c r="E13" s="35">
+      <c r="E13" s="18">
         <v>17</v>
       </c>
-      <c r="F13" s="35">
+      <c r="F13" s="18">
         <v>3</v>
       </c>
-      <c r="G13" s="36">
+      <c r="G13" s="19">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="2:186" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="34" t="s">
+      <c r="B14" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="35">
+      <c r="C14" s="18">
         <v>19</v>
       </c>
-      <c r="D14" s="35">
+      <c r="D14" s="18">
         <v>3</v>
       </c>
-      <c r="E14" s="35">
+      <c r="E14" s="18">
         <v>19</v>
       </c>
-      <c r="F14" s="35">
+      <c r="F14" s="18">
         <v>3</v>
       </c>
-      <c r="G14" s="36">
+      <c r="G14" s="19">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="2:186" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="34" t="s">
+      <c r="B15" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="35">
+      <c r="C15" s="18">
         <v>23</v>
       </c>
-      <c r="D15" s="35">
+      <c r="D15" s="18">
         <v>3</v>
       </c>
-      <c r="E15" s="35">
+      <c r="E15" s="18">
         <v>23</v>
       </c>
-      <c r="F15" s="35">
+      <c r="F15" s="18">
         <v>3</v>
       </c>
-      <c r="G15" s="36">
+      <c r="G15" s="19">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="2:186" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="34" t="s">
+      <c r="B16" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="35">
+      <c r="C16" s="18">
         <v>27</v>
       </c>
-      <c r="D16" s="35">
+      <c r="D16" s="18">
         <v>3</v>
       </c>
-      <c r="E16" s="35">
+      <c r="E16" s="18">
         <v>27</v>
       </c>
-      <c r="F16" s="35">
+      <c r="F16" s="18">
         <v>3</v>
       </c>
-      <c r="G16" s="36">
+      <c r="G16" s="19">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="34" t="s">
+      <c r="B17" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="35">
+      <c r="C17" s="18">
         <v>30</v>
       </c>
-      <c r="D17" s="35">
+      <c r="D17" s="18">
         <v>18</v>
       </c>
-      <c r="E17" s="35">
+      <c r="E17" s="18">
         <v>30</v>
       </c>
-      <c r="F17" s="35">
+      <c r="F17" s="18">
         <v>18</v>
       </c>
-      <c r="G17" s="36">
+      <c r="G17" s="19">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="34" t="s">
+      <c r="B18" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="35">
+      <c r="C18" s="18">
         <v>30</v>
       </c>
-      <c r="D18" s="35">
+      <c r="D18" s="18">
         <v>4</v>
       </c>
-      <c r="E18" s="35">
+      <c r="E18" s="18">
         <v>30</v>
       </c>
-      <c r="F18" s="35">
+      <c r="F18" s="18">
         <v>4</v>
       </c>
-      <c r="G18" s="36">
+      <c r="G18" s="19">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="34" t="s">
+      <c r="B19" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="C19" s="35">
+      <c r="C19" s="18">
         <v>35</v>
       </c>
-      <c r="D19" s="35">
+      <c r="D19" s="18">
         <v>4</v>
       </c>
-      <c r="E19" s="35">
+      <c r="E19" s="18">
         <v>35</v>
       </c>
-      <c r="F19" s="35">
+      <c r="F19" s="18">
         <v>3</v>
       </c>
-      <c r="G19" s="36">
+      <c r="G19" s="19">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="34" t="s">
+      <c r="B20" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="C20" s="35">
+      <c r="C20" s="18">
         <v>39</v>
       </c>
-      <c r="D20" s="35">
+      <c r="D20" s="18">
         <v>6</v>
       </c>
-      <c r="E20" s="35">
+      <c r="E20" s="18">
         <v>39</v>
       </c>
-      <c r="F20" s="35">
+      <c r="F20" s="18">
         <v>6</v>
       </c>
-      <c r="G20" s="36">
+      <c r="G20" s="19">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="34" t="s">
+      <c r="B21" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="C21" s="35">
+      <c r="C21" s="18">
         <v>35</v>
       </c>
-      <c r="D21" s="35">
+      <c r="D21" s="18">
         <v>4</v>
       </c>
-      <c r="E21" s="35">
+      <c r="E21" s="18">
         <v>35</v>
       </c>
-      <c r="F21" s="35">
+      <c r="F21" s="18">
         <v>4</v>
       </c>
-      <c r="G21" s="36">
+      <c r="G21" s="19">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="34" t="s">
+      <c r="B22" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="C22" s="35">
+      <c r="C22" s="18">
         <v>48</v>
       </c>
-      <c r="D22" s="35">
+      <c r="D22" s="18">
         <v>77</v>
       </c>
-      <c r="E22" s="35">
+      <c r="E22" s="18">
         <v>45</v>
       </c>
-      <c r="F22" s="35"/>
-      <c r="G22" s="36">
+      <c r="F22" s="18">
+        <v>78</v>
+      </c>
+      <c r="G22" s="19">
         <v>0.5</v>
       </c>
     </row>
     <row r="23" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="34" t="s">
+      <c r="B23" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="C23" s="35">
+      <c r="C23" s="18">
         <v>46</v>
       </c>
-      <c r="D23" s="35">
+      <c r="D23" s="18">
         <v>49</v>
       </c>
-      <c r="E23" s="35">
+      <c r="E23" s="18">
         <v>46</v>
       </c>
-      <c r="F23" s="35"/>
-      <c r="G23" s="36">
+      <c r="F23" s="18">
+        <v>46</v>
+      </c>
+      <c r="G23" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B24" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" s="18">
+        <v>46</v>
+      </c>
+      <c r="D24" s="18">
+        <v>49</v>
+      </c>
+      <c r="E24" s="18">
+        <v>46</v>
+      </c>
+      <c r="F24" s="18">
+        <v>46</v>
+      </c>
+      <c r="G24" s="19">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B25" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" s="18">
+        <v>95</v>
+      </c>
+      <c r="D25" s="18">
+        <v>15</v>
+      </c>
+      <c r="E25" s="18">
+        <v>96</v>
+      </c>
+      <c r="F25" s="18">
+        <v>16</v>
+      </c>
+      <c r="G25" s="19">
         <v>0.5</v>
       </c>
     </row>
-    <row r="24" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="34" t="s">
-        <v>32</v>
-      </c>
-      <c r="C24" s="35">
-        <v>46</v>
-      </c>
-      <c r="D24" s="35">
-        <v>49</v>
-      </c>
-      <c r="E24" s="35">
-        <v>46</v>
-      </c>
-      <c r="F24" s="35"/>
-      <c r="G24" s="36">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="25" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="34" t="s">
-        <v>26</v>
-      </c>
-      <c r="C25" s="35">
-        <v>95</v>
-      </c>
-      <c r="D25" s="35">
-        <v>30</v>
-      </c>
-      <c r="E25" s="35"/>
-      <c r="F25" s="35"/>
-      <c r="G25" s="36">
+    <row r="26" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B26" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26" s="18">
+        <v>125</v>
+      </c>
+      <c r="D26" s="18">
+        <v>7</v>
+      </c>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="19">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="C26" s="35">
-        <v>125</v>
-      </c>
-      <c r="D26" s="35">
-        <v>7</v>
-      </c>
-      <c r="E26" s="35"/>
-      <c r="F26" s="35"/>
-      <c r="G26" s="36">
-        <v>0</v>
-      </c>
-    </row>
     <row r="27" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="34" t="s">
+      <c r="B27" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="C27" s="35">
+      <c r="C27" s="18">
+        <v>1</v>
+      </c>
+      <c r="D27" s="18">
         <v>137</v>
       </c>
-      <c r="D27" s="35">
+      <c r="E27" s="18">
+        <v>1</v>
+      </c>
+      <c r="F27" s="18">
         <v>137</v>
       </c>
-      <c r="E27" s="35"/>
-      <c r="F27" s="35"/>
-      <c r="G27" s="36">
-        <v>0.09</v>
+      <c r="G27" s="19">
+        <v>0.9</v>
       </c>
     </row>
     <row r="28" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="37"/>
-      <c r="C28" s="38"/>
-      <c r="D28" s="38"/>
-      <c r="E28" s="38"/>
-      <c r="F28" s="38"/>
-      <c r="G28" s="36"/>
+      <c r="B28" s="20"/>
+      <c r="C28" s="21"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="21"/>
+      <c r="G28" s="19"/>
     </row>
     <row r="29" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B29" s="37"/>
-      <c r="C29" s="38"/>
-      <c r="D29" s="38"/>
-      <c r="E29" s="38"/>
-      <c r="F29" s="38"/>
-      <c r="G29" s="36"/>
+      <c r="B29" s="20"/>
+      <c r="C29" s="21"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="21"/>
+      <c r="F29" s="21"/>
+      <c r="G29" s="19"/>
     </row>
     <row r="30" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B30" s="37"/>
-      <c r="C30" s="38"/>
-      <c r="D30" s="38"/>
-      <c r="E30" s="38"/>
-      <c r="F30" s="38"/>
-      <c r="G30" s="36"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="21"/>
+      <c r="F30" s="21"/>
+      <c r="G30" s="19"/>
     </row>
     <row r="31" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B31" s="37"/>
-      <c r="C31" s="38"/>
-      <c r="D31" s="38"/>
-      <c r="E31" s="38"/>
-      <c r="F31" s="38"/>
-      <c r="G31" s="36"/>
+      <c r="B31" s="20"/>
+      <c r="C31" s="21"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="21"/>
+      <c r="G31" s="19"/>
     </row>
     <row r="32" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="37"/>
-      <c r="C32" s="38"/>
-      <c r="D32" s="38"/>
-      <c r="E32" s="38"/>
-      <c r="F32" s="38"/>
-      <c r="G32" s="36"/>
+      <c r="B32" s="20"/>
+      <c r="C32" s="21"/>
+      <c r="D32" s="21"/>
+      <c r="E32" s="21"/>
+      <c r="F32" s="21"/>
+      <c r="G32" s="19"/>
     </row>
     <row r="33" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B33" s="37"/>
-      <c r="C33" s="38"/>
-      <c r="D33" s="38"/>
-      <c r="E33" s="38"/>
-      <c r="F33" s="38"/>
-      <c r="G33" s="36"/>
+      <c r="B33" s="20"/>
+      <c r="C33" s="21"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="21"/>
+      <c r="F33" s="21"/>
+      <c r="G33" s="19"/>
     </row>
     <row r="34" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B34" s="37"/>
-      <c r="C34" s="38"/>
-      <c r="D34" s="38"/>
-      <c r="E34" s="38"/>
-      <c r="F34" s="38"/>
-      <c r="G34" s="36"/>
+      <c r="B34" s="20"/>
+      <c r="C34" s="21"/>
+      <c r="D34" s="21"/>
+      <c r="E34" s="21"/>
+      <c r="F34" s="21"/>
+      <c r="G34" s="19"/>
     </row>
     <row r="35" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B35" s="37"/>
-      <c r="C35" s="38"/>
-      <c r="D35" s="38"/>
-      <c r="E35" s="38"/>
-      <c r="F35" s="38"/>
-      <c r="G35" s="36"/>
+      <c r="B35" s="20"/>
+      <c r="C35" s="21"/>
+      <c r="D35" s="21"/>
+      <c r="E35" s="21"/>
+      <c r="F35" s="21"/>
+      <c r="G35" s="19"/>
     </row>
     <row r="36" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B36" s="37"/>
-      <c r="C36" s="38"/>
-      <c r="D36" s="38"/>
-      <c r="E36" s="38"/>
-      <c r="F36" s="38"/>
-      <c r="G36" s="36"/>
+      <c r="B36" s="20"/>
+      <c r="C36" s="21"/>
+      <c r="D36" s="21"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="21"/>
+      <c r="G36" s="19"/>
     </row>
     <row r="37" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B37" s="37"/>
-      <c r="C37" s="38"/>
-      <c r="D37" s="38"/>
-      <c r="E37" s="38"/>
-      <c r="F37" s="38"/>
-      <c r="G37" s="36"/>
+      <c r="B37" s="20"/>
+      <c r="C37" s="21"/>
+      <c r="D37" s="21"/>
+      <c r="E37" s="21"/>
+      <c r="F37" s="21"/>
+      <c r="G37" s="19"/>
     </row>
     <row r="38" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B38" s="37"/>
-      <c r="C38" s="38"/>
-      <c r="D38" s="38"/>
-      <c r="E38" s="38"/>
-      <c r="F38" s="38"/>
-      <c r="G38" s="36"/>
+      <c r="B38" s="20"/>
+      <c r="C38" s="21"/>
+      <c r="D38" s="21"/>
+      <c r="E38" s="21"/>
+      <c r="F38" s="21"/>
+      <c r="G38" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="12">

</xml_diff>

<commit_message>
Added introduction to technical manual
</commit_message>
<xml_diff>
--- a/FYP documentation/FYP_Project_Plan.xlsx
+++ b/FYP documentation/FYP_Project_Plan.xlsx
@@ -1133,8 +1133,8 @@
   </sheetPr>
   <dimension ref="B1:GD38"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" zoomScale="59" zoomScaleNormal="59" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="59" zoomScaleNormal="59" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="Q19" sqref="Q19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1827,7 +1827,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:186" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:186" ht="47.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="17" t="s">
         <v>15</v>
       </c>
@@ -1847,7 +1847,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:186" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:186" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="17" t="s">
         <v>16</v>
       </c>
@@ -1867,7 +1867,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:186" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:186" ht="39" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="17" t="s">
         <v>17</v>
       </c>
@@ -1887,7 +1887,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:186" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:186" ht="43.2" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="17" t="s">
         <v>18</v>
       </c>
@@ -1907,7 +1907,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:186" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:186" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="17" t="s">
         <v>23</v>
       </c>
@@ -1927,7 +1927,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:186" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:186" ht="46.2" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="17" t="s">
         <v>19</v>
       </c>
@@ -1947,7 +1947,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:186" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:186" ht="43.2" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="17" t="s">
         <v>20</v>
       </c>
@@ -1967,7 +1967,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:186" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:186" ht="62.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="17" t="s">
         <v>21</v>
       </c>
@@ -1987,7 +1987,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:186" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:186" ht="71.400000000000006" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="17" t="s">
         <v>24</v>
       </c>
@@ -2007,7 +2007,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:186" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:186" ht="64.8" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="17" t="s">
         <v>29</v>
       </c>
@@ -2027,7 +2027,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="2:186" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:186" ht="43.2" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="17" t="s">
         <v>30</v>
       </c>
@@ -2067,7 +2067,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:7" ht="50.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B18" s="17" t="s">
         <v>36</v>
       </c>
@@ -2087,7 +2087,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:7" ht="42" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B19" s="17" t="s">
         <v>33</v>
       </c>
@@ -2107,7 +2107,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:7" ht="42" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B20" s="17" t="s">
         <v>34</v>
       </c>
@@ -2127,7 +2127,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:7" ht="43.2" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B21" s="17" t="s">
         <v>35</v>
       </c>
@@ -2164,7 +2164,7 @@
         <v>78</v>
       </c>
       <c r="G22" s="19">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
@@ -2204,7 +2204,7 @@
         <v>46</v>
       </c>
       <c r="G24" s="19">
-        <v>0.9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
@@ -2224,7 +2224,7 @@
         <v>16</v>
       </c>
       <c r="G25" s="19">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
@@ -2237,10 +2237,12 @@
       <c r="D26" s="18">
         <v>7</v>
       </c>
-      <c r="E26" s="18"/>
+      <c r="E26" s="18">
+        <v>128</v>
+      </c>
       <c r="F26" s="18"/>
       <c r="G26" s="19">
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="27" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Made some chnages to technical manual and made precentation
</commit_message>
<xml_diff>
--- a/FYP documentation/FYP_Project_Plan.xlsx
+++ b/FYP documentation/FYP_Project_Plan.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18528"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18625"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -1133,8 +1133,8 @@
   </sheetPr>
   <dimension ref="B1:GD38"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="49" zoomScaleNormal="49" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:F27"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScale="49" zoomScaleNormal="49" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1143,8 +1143,10 @@
     <col min="2" max="2" width="36.6640625" style="22" customWidth="1"/>
     <col min="3" max="6" width="11.6640625" style="3" customWidth="1"/>
     <col min="7" max="7" width="15.6640625" style="23" customWidth="1"/>
-    <col min="8" max="8" width="3.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="23" width="2.77734375" style="3"/>
+    <col min="8" max="8" width="8.33203125" style="3" customWidth="1"/>
+    <col min="9" max="16" width="2.77734375" style="3"/>
+    <col min="17" max="17" width="4.21875" style="3" bestFit="1" customWidth="1"/>
+    <col min="18" max="23" width="2.77734375" style="3"/>
     <col min="24" max="24" width="12" style="3" customWidth="1"/>
     <col min="25" max="27" width="2.77734375" style="3"/>
     <col min="28" max="33" width="2.77734375" style="4"/>
@@ -1174,7 +1176,7 @@
         <v>5</v>
       </c>
       <c r="H2" s="6">
-        <v>85</v>
+        <v>132</v>
       </c>
       <c r="J2" s="7"/>
       <c r="K2" s="33" t="s">
@@ -2235,14 +2237,16 @@
         <v>125</v>
       </c>
       <c r="D26" s="18">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E26" s="18">
         <v>128</v>
       </c>
-      <c r="F26" s="18"/>
+      <c r="F26" s="18">
+        <v>3</v>
+      </c>
       <c r="G26" s="19">
-        <v>0.2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
@@ -2253,16 +2257,16 @@
         <v>1</v>
       </c>
       <c r="D27" s="18">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="E27" s="18">
         <v>1</v>
       </c>
       <c r="F27" s="18">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="G27" s="19">
-        <v>0.9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">

</xml_diff>